<commit_message>
Update conventional models (partially)
</commit_message>
<xml_diff>
--- a/params/context.xlsx
+++ b/params/context.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -28,6 +28,12 @@
     <t xml:space="preserve">value1</t>
   </si>
   <si>
+    <t xml:space="preserve">lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper</t>
+  </si>
+  <si>
     <t xml:space="preserve">notes</t>
   </si>
   <si>
@@ -37,16 +43,13 @@
     <t xml:space="preserve">Tarifa ICS 2013</t>
   </si>
   <si>
-    <t xml:space="preserve">c_cyto_arnm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_cyto_hpvhc</t>
+    <t xml:space="preserve">c_cyto_hpv16_la</t>
   </si>
   <si>
     <t xml:space="preserve">Lam 2011 (assuming c_cyto + c_hpv)</t>
   </si>
   <si>
-    <t xml:space="preserve">c_cyto_hpvla</t>
+    <t xml:space="preserve">c_hpv16_la</t>
   </si>
   <si>
     <t xml:space="preserve">c_followup</t>
@@ -55,12 +58,6 @@
     <t xml:space="preserve">* (semestral followups)</t>
   </si>
   <si>
-    <t xml:space="preserve">c_followup__irc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goldie 2000 (Treatment cost hsil)</t>
-  </si>
-  <si>
     <t xml:space="preserve">c_hra</t>
   </si>
   <si>
@@ -71,6 +68,42 @@
   </si>
   <si>
     <t xml:space="preserve">Tarifa ICS 2013 (mid range value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivity_hpv16_la</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specificity_hpv16_la</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivity_hra___cyto_no_hsil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specificity_hra___cyto_no_hsil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivity_hra___cyto_hsil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specificity_hra___cyto_hsil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_hra_hsil___cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_hra_hsil___no_cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_cyto_b___cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_cyto_b___no_cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_cyto_hsil___cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_cyto_hsil___no_cancer</t>
   </si>
   <si>
     <t xml:space="preserve">u_hiv_p</t>
@@ -197,17 +230,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="85.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -220,103 +254,154 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
+      <c r="C2" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0</v>
+        <f aca="false">B4+B2</f>
+        <v>171</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
-        <f aca="false">95+B2</f>
-        <v>171</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <f aca="false">95+B2</f>
-        <v>171</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>10</v>
+        <v>225</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>2483</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>8213</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>225</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>14</v>
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>8213</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>0.6</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.94</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>18</v>
+        <v>0.8</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,21 +409,176 @@
         <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>0.7</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>-1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B13" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="0" t="n">
         <v>0.84</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
+      <c r="C22" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update sens/spec parameters with ELAVI info
</commit_message>
<xml_diff>
--- a/params/context.xlsx
+++ b/params/context.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\david\anus\params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9932F780-0A53-4CBC-9291-D29409A80F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF51A71-43A7-41FC-8862-5FD11DAD92FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7140" windowWidth="18240" windowHeight="29040" tabRatio="801" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="113">
   <si>
     <t>variable</t>
   </si>
@@ -157,24 +157,6 @@
     <t>ELAVI [0/197]</t>
   </si>
   <si>
-    <t>ELAVI [1-65/210]</t>
-  </si>
-  <si>
-    <t>ELAVI [1-0/7]</t>
-  </si>
-  <si>
-    <t>ELAVI [1-17/141]</t>
-  </si>
-  <si>
-    <t>ELAVI [1-59/156]</t>
-  </si>
-  <si>
-    <t>ELAVI [1-48/126]</t>
-  </si>
-  <si>
-    <t>ELAVI [1-13/119]</t>
-  </si>
-  <si>
     <t>Tarifa ICS 2013 (mid range value) [Anna]</t>
   </si>
   <si>
@@ -391,30 +373,6 @@
     <t>p_hsil_regression_annual</t>
   </si>
   <si>
-    <t>ELAVI [48/157]</t>
-  </si>
-  <si>
-    <t>ELAVI [58/157]</t>
-  </si>
-  <si>
-    <t>ELAVI [114/157]</t>
-  </si>
-  <si>
-    <t>ELAVI [66/157]</t>
-  </si>
-  <si>
-    <t>ELAVI [74/157]</t>
-  </si>
-  <si>
-    <t>ELAVI [135/157]</t>
-  </si>
-  <si>
-    <t>ELAVI [88/157]</t>
-  </si>
-  <si>
-    <t>ELAVI [1-79/241]</t>
-  </si>
-  <si>
     <t>p_no_hsil___hsil_irc</t>
   </si>
   <si>
@@ -425,6 +383,9 @@
   </si>
   <si>
     <t>Assuming previous IRC does not prevent future HSILs</t>
+  </si>
+  <si>
+    <t>ELAVI descriptive statistics</t>
   </si>
 </sst>
 </file>
@@ -494,15 +455,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -836,7 +796,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -862,11 +822,11 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="4">
@@ -879,11 +839,11 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="4">
@@ -896,11 +856,11 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="4">
@@ -913,7 +873,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -988,7 +948,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B11">
         <f>B10+B14</f>
@@ -1006,7 +966,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>75.53</v>
@@ -1018,12 +978,12 @@
         <v>-1</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4">
         <v>24.56</v>
@@ -1035,12 +995,12 @@
         <v>-1</v>
       </c>
       <c r="E13" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B14">
         <v>31.6</v>
@@ -1052,7 +1012,7 @@
         <v>-1</v>
       </c>
       <c r="E14" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1069,12 +1029,12 @@
         <v>-1</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B16">
         <f>1-(1-B17)^(1/$B$77)</f>
@@ -1089,9 +1049,9 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="6">
+        <v>85</v>
+      </c>
+      <c r="B17">
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="C17">
@@ -1101,12 +1061,12 @@
         <v>-1</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>51</v>
+      <c r="A18" t="s">
+        <v>45</v>
       </c>
       <c r="B18">
         <v>0.40129999999999999</v>
@@ -1122,8 +1082,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>61</v>
+      <c r="A19" t="s">
+        <v>55</v>
       </c>
       <c r="B19">
         <v>0.2792</v>
@@ -1139,8 +1099,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>52</v>
+      <c r="A20" t="s">
+        <v>46</v>
       </c>
       <c r="B20">
         <v>0.27389999999999998</v>
@@ -1156,8 +1116,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>62</v>
+      <c r="A21" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B21">
         <v>0.64470000000000005</v>
@@ -1173,8 +1133,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>53</v>
+      <c r="A22" t="s">
+        <v>47</v>
       </c>
       <c r="B22">
         <v>0.30570000000000003</v>
@@ -1190,8 +1150,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>63</v>
+      <c r="A23" t="s">
+        <v>57</v>
       </c>
       <c r="B23">
         <v>2.5399999999999999E-2</v>
@@ -1238,7 +1198,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B26" s="3">
         <v>0.01</v>
@@ -1250,236 +1210,236 @@
         <v>-1</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="C27">
+        <v>-1</v>
+      </c>
+      <c r="D27">
+        <v>-1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28">
+        <v>9.2600000000000002E-2</v>
+      </c>
+      <c r="C28">
+        <v>-1</v>
+      </c>
+      <c r="D28">
+        <v>-1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="C29">
+        <v>-1</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="C30">
+        <v>-1</v>
+      </c>
+      <c r="D30">
+        <v>-1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="C31">
+        <v>-1</v>
+      </c>
+      <c r="D31">
+        <v>-1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="C32">
+        <v>-1</v>
+      </c>
+      <c r="D32">
+        <v>-1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33">
+        <v>0.432</v>
+      </c>
+      <c r="C33">
+        <v>-1</v>
+      </c>
+      <c r="D33">
+        <v>-1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C34">
+        <v>-1</v>
+      </c>
+      <c r="D34">
+        <v>-1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="C35">
+        <v>-1</v>
+      </c>
+      <c r="D35">
+        <v>-1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="C36">
+        <v>-1</v>
+      </c>
+      <c r="D36">
+        <v>-1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="C37">
+        <v>-1</v>
+      </c>
+      <c r="D37">
+        <v>-1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="C38">
+        <v>-1</v>
+      </c>
+      <c r="D38">
+        <v>-1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>54</v>
       </c>
-      <c r="B27">
-        <v>0.30570000000000003</v>
-      </c>
-      <c r="C27">
-        <v>-1</v>
-      </c>
-      <c r="D27">
-        <v>-1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="B39">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="C39">
+        <v>-1</v>
+      </c>
+      <c r="D39">
+        <v>-1</v>
+      </c>
+      <c r="E39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="6">
-        <v>0.62180000000000002</v>
-      </c>
-      <c r="C28">
-        <v>-1</v>
-      </c>
-      <c r="D28">
-        <v>-1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29">
-        <v>0.36940000000000001</v>
-      </c>
-      <c r="C29">
-        <v>-1</v>
-      </c>
-      <c r="D29">
-        <v>-1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="6">
-        <v>0.61899999999999999</v>
-      </c>
-      <c r="C30">
-        <v>-1</v>
-      </c>
-      <c r="D30">
-        <v>-1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31">
-        <v>0.72609999999999997</v>
-      </c>
-      <c r="C31">
-        <v>-1</v>
-      </c>
-      <c r="D31">
-        <v>-1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="6">
-        <v>0.89080000000000004</v>
-      </c>
-      <c r="C32">
-        <v>-1</v>
-      </c>
-      <c r="D32">
-        <v>-1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33">
-        <v>0.4204</v>
-      </c>
-      <c r="C33">
-        <v>-1</v>
-      </c>
-      <c r="D33">
-        <v>-1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="6">
-        <v>0.67220000000000002</v>
-      </c>
-      <c r="C34">
-        <v>-1</v>
-      </c>
-      <c r="D34">
-        <v>-1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35">
-        <v>0.4713</v>
-      </c>
-      <c r="C35">
-        <v>-1</v>
-      </c>
-      <c r="D35">
-        <v>-1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="6">
-        <v>0.6905</v>
-      </c>
-      <c r="C36">
-        <v>-1</v>
-      </c>
-      <c r="D36">
-        <v>-1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37">
-        <v>0.8599</v>
-      </c>
-      <c r="C37">
-        <v>-1</v>
-      </c>
-      <c r="D37">
-        <v>-1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="6">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>-1</v>
-      </c>
-      <c r="D38">
-        <v>-1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39">
-        <v>0.5605</v>
-      </c>
-      <c r="C39">
-        <v>-1</v>
-      </c>
-      <c r="D39">
-        <v>-1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="6">
-        <v>0.87939999999999996</v>
+      <c r="B40">
+        <v>0.33</v>
       </c>
       <c r="C40">
         <v>-1</v>
@@ -1488,12 +1448,12 @@
         <v>-1</v>
       </c>
       <c r="E40" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B41">
         <v>0.85350000000000004</v>
@@ -1510,7 +1470,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B42" s="4">
         <v>0</v>
@@ -1522,12 +1482,12 @@
         <v>-1</v>
       </c>
       <c r="E42" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B43">
         <f>B41</f>
@@ -1545,7 +1505,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B44" s="4">
         <f>B42</f>
@@ -1562,8 +1522,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
-        <v>75</v>
+      <c r="A45" t="s">
+        <v>69</v>
       </c>
       <c r="B45" s="4">
         <v>7.6299999999999996E-3</v>
@@ -1575,12 +1535,12 @@
         <v>-1</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>76</v>
+      <c r="A46" t="s">
+        <v>70</v>
       </c>
       <c r="B46" s="4">
         <v>0</v>
@@ -1596,8 +1556,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
-        <v>77</v>
+      <c r="A47" t="s">
+        <v>71</v>
       </c>
       <c r="B47" s="4">
         <f>B45</f>
@@ -1610,12 +1570,12 @@
         <v>-1</v>
       </c>
       <c r="E47" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>78</v>
+      <c r="A48" t="s">
+        <v>72</v>
       </c>
       <c r="B48" s="4">
         <f>B46</f>
@@ -1633,9 +1593,9 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>110</v>
-      </c>
-      <c r="B49" s="6">
+        <v>104</v>
+      </c>
+      <c r="B49">
         <f>1-(1-B52)^(1/$B$77)</f>
         <v>0.22798963737524869</v>
       </c>
@@ -1648,9 +1608,9 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" s="6">
+        <v>105</v>
+      </c>
+      <c r="B50">
         <f>B49</f>
         <v>0.22798963737524869</v>
       </c>
@@ -1663,9 +1623,9 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>112</v>
-      </c>
-      <c r="B51" s="6">
+        <v>106</v>
+      </c>
+      <c r="B51">
         <f>B66*(1-B25)</f>
         <v>0.99498743710661997</v>
       </c>
@@ -1678,9 +1638,9 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="6">
+        <v>107</v>
+      </c>
+      <c r="B52">
         <v>0.40400000000000003</v>
       </c>
       <c r="C52">
@@ -1690,12 +1650,12 @@
         <v>-1</v>
       </c>
       <c r="E52" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B53" s="4">
         <f>1-(1-B56)^(1/$B$77)</f>
@@ -1710,7 +1670,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B54" s="4">
         <f>B53*B67</f>
@@ -1723,14 +1683,14 @@
         <v>-1</v>
       </c>
       <c r="E54" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>80</v>
-      </c>
-      <c r="B55" s="6">
+        <v>74</v>
+      </c>
+      <c r="B55">
         <f>B53</f>
         <v>5.2793581102830611E-2</v>
       </c>
@@ -1743,9 +1703,9 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>99</v>
-      </c>
-      <c r="B56" s="6">
+        <v>93</v>
+      </c>
+      <c r="B56">
         <v>0.1028</v>
       </c>
       <c r="C56">
@@ -1755,14 +1715,14 @@
         <v>-1</v>
       </c>
       <c r="E56" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>104</v>
-      </c>
-      <c r="B57" s="6">
+        <v>98</v>
+      </c>
+      <c r="B57">
         <f>1-EXP(-(-LOG(B60,EXP(1))/17.5)*1/$B$77)</f>
         <v>2.9549534482222528E-2</v>
       </c>
@@ -1775,9 +1735,9 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>105</v>
-      </c>
-      <c r="B58" s="6">
+        <v>99</v>
+      </c>
+      <c r="B58">
         <f>B57*B67</f>
         <v>2.9549534482222528E-2</v>
       </c>
@@ -1790,9 +1750,9 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" s="6">
+        <v>100</v>
+      </c>
+      <c r="B59">
         <f>B57</f>
         <v>2.9549534482222528E-2</v>
       </c>
@@ -1805,7 +1765,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B60" s="4">
         <v>0.35</v>
@@ -1817,14 +1777,14 @@
         <v>-1</v>
       </c>
       <c r="E60" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>13</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61">
         <f>1-(1-B62)^(1/$B$77)</f>
         <v>0</v>
       </c>
@@ -1837,7 +1797,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B62" s="3">
         <v>0</v>
@@ -1849,12 +1809,12 @@
         <v>-1</v>
       </c>
       <c r="E62" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B63" s="3">
         <v>0</v>
@@ -1866,12 +1826,12 @@
         <v>-1</v>
       </c>
       <c r="E63" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B64">
         <v>0.71499999999999997</v>
@@ -1883,12 +1843,12 @@
         <v>-1</v>
       </c>
       <c r="E64" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B65" s="3">
         <v>1</v>
@@ -1900,12 +1860,12 @@
         <v>-1</v>
       </c>
       <c r="E65" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B66" s="3">
         <v>1</v>
@@ -1917,12 +1877,12 @@
         <v>-1</v>
       </c>
       <c r="E66" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B67" s="3">
         <v>1</v>
@@ -1934,7 +1894,7 @@
         <v>-1</v>
       </c>
       <c r="E67" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -1951,12 +1911,12 @@
         <v>0.86</v>
       </c>
       <c r="E68" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B69" s="3">
         <f>B68</f>
@@ -1971,9 +1931,9 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>49</v>
-      </c>
-      <c r="B70" s="6">
+        <v>43</v>
+      </c>
+      <c r="B70">
         <f>0.98*B68</f>
         <v>0.74480000000000002</v>
       </c>
@@ -1986,7 +1946,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B71" s="3">
         <f>0.98*B69</f>
@@ -2013,7 +1973,7 @@
         <v>0.7</v>
       </c>
       <c r="E72" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2031,7 +1991,7 @@
         <v>-1</v>
       </c>
       <c r="E73" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2049,12 +2009,12 @@
         <v>-1</v>
       </c>
       <c r="E74" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B75" s="4">
         <v>0.7</v>
@@ -2144,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2158,9 +2118,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="C2">
@@ -2170,12 +2130,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.69699999999999995</v>
@@ -2187,12 +2147,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -2204,14 +2164,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C5">
@@ -2221,7 +2181,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2249,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2263,9 +2223,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="C2">
@@ -2275,12 +2235,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.68500000000000005</v>
@@ -2292,12 +2252,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -2309,14 +2269,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C5">
@@ -2326,7 +2286,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2354,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2368,9 +2328,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="C2">
@@ -2380,12 +2340,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.68500000000000005</v>
@@ -2397,12 +2357,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -2414,14 +2374,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C5">
@@ -2431,7 +2391,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2459,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2473,9 +2433,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="C2">
@@ -2485,12 +2445,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.71499999999999997</v>
@@ -2502,12 +2462,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -2519,14 +2479,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>0.40400000000000003</v>
       </c>
       <c r="C5">
@@ -2536,7 +2496,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2565,7 +2525,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2579,9 +2539,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="C2">
@@ -2591,12 +2551,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.71499999999999997</v>
@@ -2608,12 +2568,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -2625,14 +2585,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>0.314</v>
       </c>
       <c r="C5">
@@ -2642,7 +2602,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2670,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2684,9 +2644,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>1.0580000000000001E-2</v>
       </c>
       <c r="C2">
@@ -2696,12 +2656,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.71499999999999997</v>
@@ -2713,12 +2673,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -2730,14 +2690,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>0.314</v>
       </c>
       <c r="C5">
@@ -2747,7 +2707,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2775,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2789,9 +2749,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>1.0580000000000001E-2</v>
       </c>
       <c r="C2">
@@ -2801,12 +2761,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.71099999999999997</v>
@@ -2818,12 +2778,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -2835,14 +2795,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>0.219</v>
       </c>
       <c r="C5">
@@ -2852,7 +2812,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2880,7 +2840,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2894,9 +2854,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="C2">
@@ -2906,12 +2866,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.71099999999999997</v>
@@ -2923,12 +2883,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -2940,14 +2900,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>0.219</v>
       </c>
       <c r="C5">
@@ -2957,7 +2917,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2985,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2999,9 +2959,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="C2">
@@ -3011,12 +2971,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.70299999999999996</v>
@@ -3028,12 +2988,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -3045,14 +3005,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C5">
@@ -3062,7 +3022,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3090,7 +3050,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3104,9 +3064,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="C2">
@@ -3116,12 +3076,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.70299999999999996</v>
@@ -3133,12 +3093,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -3150,14 +3110,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C5">
@@ -3167,7 +3127,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -3195,7 +3155,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3209,9 +3169,9 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="6">
+        <v>85</v>
+      </c>
+      <c r="B2">
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="C2">
@@ -3221,12 +3181,12 @@
         <v>-1</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>0.69699999999999995</v>
@@ -3238,12 +3198,12 @@
         <v>-1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>1.7060000000000001E-3</v>
@@ -3255,14 +3215,14 @@
         <v>-1</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="6">
+        <v>107</v>
+      </c>
+      <c r="B5">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C5">
@@ -3272,7 +3232,7 @@
         <v>-1</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix sensitivity analysis and calibration code, add context metadata support
</commit_message>
<xml_diff>
--- a/params/context.xlsx
+++ b/params/context.xlsx
@@ -21,6 +21,9 @@
     <sheet name="y75_79" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="y80_84" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">y25_29!$A$1:$G$88</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="188">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -48,12 +51,21 @@
     <t xml:space="preserve">notes</t>
   </si>
   <si>
+    <t xml:space="preserve">display_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_cyto</t>
   </si>
   <si>
     <t xml:space="preserve">Inventario ELAVI</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of cytology</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_arnm16</t>
   </si>
   <si>
@@ -72,6 +84,9 @@
     <t xml:space="preserve">Inventario ELAVI [25€ (500/any) o 6€ (3000-70000/any)]</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of ARN kit</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_hpv16la</t>
   </si>
   <si>
@@ -84,12 +99,21 @@
     <t xml:space="preserve">c_hpvla</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of HPV test (LA)</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_hpvhrhc</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of HPV test (HC)</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_followup</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of followup</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_followup_irc</t>
   </si>
   <si>
@@ -105,36 +129,57 @@
     <t xml:space="preserve">Inventario ELAVI (actualizado Mireia)</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of HRA followup</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_hra_treatment</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of HRA treatment</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_tca_single</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of single application of TCA</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_tca</t>
   </si>
   <si>
     <t xml:space="preserve">c_irc</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of IRC</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_surgery</t>
   </si>
   <si>
     <t xml:space="preserve">GRD 231.01 Procediments majors sobre l'intestí gros, de complexitat menor</t>
   </si>
   <si>
+    <t xml:space="preserve">Cost of surgery</t>
+  </si>
+  <si>
     <t xml:space="preserve">n_tca</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI (Maria)</t>
   </si>
   <si>
+    <t xml:space="preserve">Mean number of TCA per patient</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_cancer___hra_invasive_cancer</t>
   </si>
   <si>
     <t xml:space="preserve">Assumption</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of AC in patients with invasive AC in HRA</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_cancer___hsil</t>
   </si>
   <si>
@@ -144,42 +189,63 @@
     <t xml:space="preserve">Deshmuk 2015 [HGAIN to anal cancer] (see deshmuk_calculations.xlsx)</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of developing AC in HSIL patients (annual)</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_cyto_ascus_or_lsil___hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI [(33+30)/157]</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of ASCUS or LSIL result in cytology in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_cyto_ascus_or_lsil___no_hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI [(24+31)/197]</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of ASCUS or LSIL result in cytology in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_cyto_b___hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI [43/157]</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of benign result in cytology in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_cyto_b___no_hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI [127/197]</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of benign result in cytology in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_cyto_hsil___hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI [(5+43)/157]</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of HSIL result in cytology in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_cyto_hsil___no_hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI [(5+0)/197]</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of HSIL result in cytology in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_death_cancer</t>
   </si>
   <si>
@@ -192,69 +258,120 @@
     <t xml:space="preserve">WHO [2016, Spain, prob death between 15-60 per 1000=74 -&gt; lambda=0.001708 -&gt; P(S&lt;1)=0.001706]</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of death from other causes (annual)</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_arnm16_p___hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI preprint (table 3)</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in ARNm-E6/E7 (16) in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_arnm16_p___no_hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in ARNm-E6/E7 (16) in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_arnm161845_p___hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI descriptive statistics (table 12, 52)</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in ARNm-E6/E7 (16/18/45) in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_arnm161845_p___no_hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in ARNm-E6/E7 (16/18/45) in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_arnmhr_p___hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in ARNm-E6/E7 (high-risk) in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_arnmhr_p___no_hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in ARNm-E6/E7 (high-risk) in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hpv16la_p___hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in HPV-LA test (16) in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hpv16la_p___no_hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in HPV-LA test (16) in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hpv1618la_p___hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in HPV-LA test (16/18) in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hpv1618la_p___no_hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in HPV-LA test (16/18) in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hpvhrla_p___hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI preprint (table 3) </t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in HPV-LA test (high-risk) in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hpvhrla_p___no_hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in HPV-LA test (high-risk) in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hpvhrhc_p___hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in HPV-HC test (high-risk) in HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hpvhrhc_p___no_hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of positive in HPV-HC test (high-risk) in no-HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hra_hsil___cyto_hsil__hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI [134/157]</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of HSIL in HRA in HSIL patients that got HSIL in cytology</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hra_hsil___cyto_hsil__no_hsil</t>
   </si>
   <si>
     <t xml:space="preserve">ELAVI [0/197] (=0?)</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of HSIL in HRA in HSIL patients that got no-HSIL in cytology</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hra_hsil___cyto_no_hsil__hsil</t>
   </si>
   <si>
@@ -273,6 +390,9 @@
     <t xml:space="preserve">p_hra_invasive_cancer___cyto_hsil__no_hsil</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of invasive cancer in HRA in no-HSIL patients that got HSIL in cytology</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hra_invasive_cancer___cyto_no_hsil__hsil</t>
   </si>
   <si>
@@ -300,6 +420,9 @@
     <t xml:space="preserve">ELAVI (aclaramiento, Ana)</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of HSIL regression (annual)</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_hsil___semestral_followup_no_hsil</t>
   </si>
   <si>
@@ -318,6 +441,9 @@
     <t xml:space="preserve">Deshmuk 2015 [Normal to HGAIN] (see deshmuk_calculations.xlsx)</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of developing HSIL (annual)</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_undetected_hsil_treatment</t>
   </si>
   <si>
@@ -327,6 +453,9 @@
     <t xml:space="preserve">Recurrencia HSIL tras tto con electrocauterización (media de seguimiento de 17.5 años): 35% (Burgos J DOI:10.1097/QAD.0000000000001433)</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of ???</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_recurrence</t>
   </si>
   <si>
@@ -336,15 +465,24 @@
     <t xml:space="preserve">???</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of recurrence (annual)</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_survive</t>
   </si>
   <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
     <t xml:space="preserve">survival_5year</t>
   </si>
   <si>
     <t xml:space="preserve">Adjusted values from SEER data (see survival_calculations.xlsx)</t>
   </si>
   <si>
+    <t xml:space="preserve">Survival rate of AC (5-year)</t>
+  </si>
+  <si>
     <t xml:space="preserve">hr_cancer_irc</t>
   </si>
   <si>
@@ -363,12 +501,18 @@
     <t xml:space="preserve">Goldstone CID 2019</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of success in IRC for HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">p_no_hsil___hsil_tca</t>
   </si>
   <si>
     <t xml:space="preserve">Goldstone CID 2019 (?)</t>
   </si>
   <si>
+    <t xml:space="preserve">Probability of success in TCA for HSIL patients</t>
+  </si>
+  <si>
     <t xml:space="preserve">hr_hsil_irc</t>
   </si>
   <si>
@@ -381,6 +525,9 @@
     <t xml:space="preserve">Deshmuk 2015</t>
   </si>
   <si>
+    <t xml:space="preserve">Utility [HIV+ MSM]</t>
+  </si>
+  <si>
     <t xml:space="preserve">u_hiv_p___irc</t>
   </si>
   <si>
@@ -399,12 +546,18 @@
     <t xml:space="preserve">u_hsil___irc</t>
   </si>
   <si>
+    <t xml:space="preserve">Utility [HSIL+IRC]</t>
+  </si>
+  <si>
     <t xml:space="preserve">u_hsil___tca</t>
   </si>
   <si>
     <t xml:space="preserve">u_cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">Utility [Anal cancer]</t>
+  </si>
+  <si>
     <t xml:space="preserve">u_sem_followup1</t>
   </si>
   <si>
@@ -417,12 +570,18 @@
     <t xml:space="preserve">u_surgery_no_cancer</t>
   </si>
   <si>
+    <t xml:space="preserve">Utility [Surgery no cancer]</t>
+  </si>
+  <si>
     <t xml:space="preserve">u_survive</t>
   </si>
   <si>
     <t xml:space="preserve">Võrno 2017</t>
   </si>
   <si>
+    <t xml:space="preserve">Utility [Survivor]</t>
+  </si>
+  <si>
     <t xml:space="preserve">periodicity_times_in_year</t>
   </si>
   <si>
@@ -433,6 +592,9 @@
   </si>
   <si>
     <t xml:space="preserve">Number of months after each simulation (period)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Periodicity</t>
   </si>
   <si>
     <t xml:space="preserve">Deshmuk 2015 [HGAIN regression] (see deshmuk_calculations.xlsx)</t>
@@ -442,11 +604,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -472,6 +635,13 @@
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -554,7 +724,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -563,7 +733,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -575,10 +757,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -587,7 +765,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -604,6 +782,57 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA9D18E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC55A11"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -667,27 +896,32 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F70" activeCellId="0" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="85.13"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="85.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="87.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,10 +937,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>10.71</v>
@@ -718,14 +958,21 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="n">
         <f aca="false">B6+0.67</f>
         <v>25.67</v>
       </c>
@@ -736,14 +983,18 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="n">
         <f aca="false">B6+0.67</f>
         <v>25.67</v>
       </c>
@@ -754,14 +1005,18 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="n">
         <f aca="false">B6+0.67</f>
         <v>25.67</v>
       </c>
@@ -772,14 +1027,18 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="n">
         <v>25</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -789,14 +1048,21 @@
         <v>-1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="n">
         <f aca="false">B10</f>
         <v>71.25</v>
       </c>
@@ -806,12 +1072,16 @@
       <c r="D7" s="0" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="n">
         <f aca="false">B10</f>
         <v>71.25</v>
       </c>
@@ -821,12 +1091,16 @@
       <c r="D8" s="0" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="n">
         <f aca="false">B10</f>
         <v>71.25</v>
       </c>
@@ -836,12 +1110,16 @@
       <c r="D9" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G9" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B9)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5" t="n">
         <v>71.25</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -849,13 +1127,20 @@
       </c>
       <c r="D10" s="0" t="n">
         <v>-1</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B10)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5" t="n">
         <v>20.02</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -863,13 +1148,20 @@
       </c>
       <c r="D11" s="0" t="n">
         <v>-1</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B11)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B12" s="6" t="n">
         <v>0</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -878,10 +1170,17 @@
       <c r="D12" s="0" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">B12+B19</f>
@@ -894,12 +1193,16 @@
         <v>-1</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B13)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">B12+B18</f>
@@ -911,12 +1214,16 @@
       <c r="D14" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G14" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B14)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7" t="n">
         <v>82.05</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -926,14 +1233,21 @@
         <v>-1</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="B16" s="7" t="n">
         <v>30.56</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -943,14 +1257,21 @@
         <v>-1</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="B17" s="7" t="n">
         <v>75.04</v>
       </c>
       <c r="C17" s="0" t="n">
@@ -960,12 +1281,19 @@
         <v>-1</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">B17*B21</f>
@@ -977,12 +1305,16 @@
       <c r="D18" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G18" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B18)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="B19" s="3" t="n">
         <v>31.6</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -992,12 +1324,19 @@
         <v>-1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B19)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3189</v>
@@ -1009,14 +1348,21 @@
         <v>-1</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B20)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="B21" s="7" t="n">
         <v>1.382</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -1026,14 +1372,21 @@
         <v>-1</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B21)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="B22" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -1043,12 +1396,19 @@
         <v>-1</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">1-(1-B24)^(1/$B$87)</f>
@@ -1060,10 +1420,14 @@
       <c r="D23" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G23" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B23)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.0036</v>
@@ -1075,12 +1439,19 @@
         <v>-1</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B24)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.4013</v>
@@ -1092,12 +1463,19 @@
         <v>-1</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>38</v>
+        <v>53</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B25)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.2792</v>
@@ -1109,12 +1487,19 @@
         <v>-1</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>40</v>
+        <v>56</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.2739</v>
@@ -1126,12 +1511,19 @@
         <v>-1</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>42</v>
+        <v>59</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G27" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>43</v>
+      <c r="A28" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0.6447</v>
@@ -1143,12 +1535,19 @@
         <v>-1</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>44</v>
+        <v>62</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.3057</v>
@@ -1160,12 +1559,19 @@
         <v>-1</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>46</v>
+        <v>65</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B29)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.0254</v>
@@ -1177,12 +1583,19 @@
         <v>-1</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>68</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">1-(1-EXP(-B70*5))^(1/$B$87)</f>
@@ -1194,10 +1607,14 @@
       <c r="D31" s="0" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>50</v>
+      <c r="G31" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B32" s="0" t="n">
         <f aca="false">1-(1-B33)^(1/$B$87)</f>
@@ -1209,12 +1626,16 @@
       <c r="D32" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G32" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B32)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B33" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C33" s="0" t="n">
@@ -1224,12 +1645,19 @@
         <v>-1</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B33)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0.386</v>
@@ -1241,12 +1669,19 @@
         <v>-1</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B34)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0.106</v>
@@ -1258,12 +1693,19 @@
         <v>-1</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B35)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0.429</v>
@@ -1275,12 +1717,19 @@
         <v>-1</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>57</v>
+        <v>81</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G36" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B36)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0.137</v>
@@ -1292,12 +1741,19 @@
         <v>-1</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>57</v>
+        <v>81</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="G37" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B37)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0.798</v>
@@ -1309,12 +1765,19 @@
         <v>-1</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>57</v>
+        <v>81</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B38)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0.404</v>
@@ -1326,12 +1789,19 @@
         <v>-1</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>57</v>
+        <v>81</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B39)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0.471</v>
@@ -1343,12 +1813,19 @@
         <v>-1</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G40" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B40)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0.173</v>
@@ -1360,12 +1837,19 @@
         <v>-1</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B41)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>0.549</v>
@@ -1377,12 +1861,19 @@
         <v>-1</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>57</v>
+        <v>81</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G42" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B42)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0.294</v>
@@ -1394,12 +1885,19 @@
         <v>-1</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>57</v>
+        <v>81</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B43)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0.94</v>
@@ -1411,12 +1909,19 @@
         <v>-1</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>66</v>
+        <v>98</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G44" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B44)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0.657</v>
@@ -1428,12 +1933,19 @@
         <v>-1</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B45)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0.757</v>
@@ -1445,12 +1957,19 @@
         <v>-1</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G46" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B46)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0.345</v>
@@ -1462,12 +1981,19 @@
         <v>-1</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B47)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>0.8535</v>
@@ -1479,12 +2005,19 @@
         <v>-1</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>71</v>
+        <v>107</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="G48" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B48)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0</v>
@@ -1496,12 +2029,19 @@
         <v>-1</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G49" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="B50" s="0" t="n">
         <f aca="false">B48</f>
@@ -1514,12 +2054,16 @@
         <v>-1</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>107</v>
+      </c>
+      <c r="G50" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B50)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="B51" s="0" t="n">
         <f aca="false">B49</f>
@@ -1532,12 +2076,16 @@
         <v>-1</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="G51" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B51)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="B52" s="0" t="n">
         <f aca="false">1/131/7.5</f>
@@ -1550,12 +2098,16 @@
         <v>-1</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>78</v>
+        <v>116</v>
+      </c>
+      <c r="G52" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B52)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -1567,12 +2119,19 @@
         <v>-1</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="G53" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="B54" s="0" t="n">
         <f aca="false">B52</f>
@@ -1585,12 +2144,16 @@
         <v>-1</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>120</v>
+      </c>
+      <c r="G54" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B54)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="B55" s="0" t="n">
         <f aca="false">B53</f>
@@ -1603,12 +2166,16 @@
         <v>-1</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+      <c r="G55" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B55)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B56" s="0" t="n">
         <f aca="false">1-(1-B60)^(1/$B$87)</f>
@@ -1620,10 +2187,14 @@
       <c r="D56" s="0" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G56" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B56)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="B57" s="0" t="n">
         <f aca="false">B56</f>
@@ -1635,10 +2206,14 @@
       <c r="D57" s="0" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G57" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B57)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="B58" s="0" t="n">
         <f aca="false">B73*(1-B32)</f>
@@ -1650,10 +2225,14 @@
       <c r="D58" s="0" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G58" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B58)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="B59" s="0" t="n">
         <f aca="false">B74*(1-B32)</f>
@@ -1665,10 +2244,14 @@
       <c r="D59" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G59" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B59)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>0.434</v>
@@ -1680,12 +2263,19 @@
         <v>-1</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>127</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="G60" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B60)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="B61" s="0" t="n">
         <f aca="false">1-(1-B64)^(1/$B$87)</f>
@@ -1697,10 +2287,14 @@
       <c r="D61" s="0" t="n">
         <v>-1</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G61" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B61)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="B62" s="0" t="n">
         <f aca="false">1-EXP(-(-LOG(B66,EXP(1))/17.5)*1/$B$87)</f>
@@ -1713,12 +2307,16 @@
         <v>-1</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>131</v>
+      </c>
+      <c r="G62" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B62)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="B63" s="0" t="n">
         <f aca="false">B61</f>
@@ -1730,10 +2328,14 @@
       <c r="D63" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G63" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B63)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>0.1028</v>
@@ -1745,12 +2347,19 @@
         <v>-1</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="G64" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B64)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="B65" s="0" t="n">
         <f aca="false">B62</f>
@@ -1762,10 +2371,14 @@
       <c r="D65" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G65" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B65)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>0.35</v>
@@ -1777,12 +2390,19 @@
         <v>-1</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>138</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="G66" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B66)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="B67" s="0" t="n">
         <f aca="false">1-(1-B68)^(1/$B$87)</f>
@@ -1794,12 +2414,16 @@
       <c r="D67" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G67" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B67)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B68" s="3" t="n">
+        <v>141</v>
+      </c>
+      <c r="B68" s="6" t="n">
         <v>0</v>
       </c>
       <c r="C68" s="0" t="n">
@@ -1809,14 +2433,21 @@
         <v>-1</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>100</v>
+        <v>142</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G68" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B68)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69" s="3" t="n">
+        <v>144</v>
+      </c>
+      <c r="B69" s="6" t="n">
         <v>0</v>
       </c>
       <c r="C69" s="0" t="n">
@@ -1826,12 +2457,19 @@
         <v>-1</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>100</v>
+        <v>142</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G69" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B69)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>0.75</v>
@@ -1843,14 +2481,21 @@
         <v>-1</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="G70" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B70)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B71" s="2" t="n">
+      <c r="A71" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="0" t="n">
@@ -1860,14 +2505,21 @@
         <v>-1</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>105</v>
+        <v>150</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G71" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B71)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="2" t="n">
+      <c r="A72" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C72" s="0" t="n">
@@ -1877,14 +2529,21 @@
         <v>-1</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>107</v>
+        <v>152</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G72" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B72)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" s="4" t="n">
+      <c r="A73" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" s="7" t="n">
         <v>0.62</v>
       </c>
       <c r="C73" s="0" t="n">
@@ -1894,14 +2553,21 @@
         <v>-1</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>109</v>
+        <v>154</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="G73" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B73)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B74" s="4" t="n">
+      <c r="A74" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B74" s="7" t="n">
         <v>0.618</v>
       </c>
       <c r="C74" s="0" t="n">
@@ -1911,14 +2577,21 @@
         <v>-1</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>111</v>
+        <v>157</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="G74" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B74)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B75" s="3" t="n">
+      <c r="A75" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B75" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C75" s="0" t="n">
@@ -1928,12 +2601,19 @@
         <v>-1</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>113</v>
+        <v>160</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G75" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B75)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>0.76</v>
@@ -1945,14 +2625,21 @@
         <v>0.86</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="G76" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B76)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B77" s="3" t="n">
+        <v>164</v>
+      </c>
+      <c r="B77" s="6" t="n">
         <f aca="false">B76</f>
         <v>0.76</v>
       </c>
@@ -1963,14 +2650,18 @@
         <v>0.86</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+      <c r="G77" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B77)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B78" s="3" t="n">
+        <v>166</v>
+      </c>
+      <c r="B78" s="6" t="n">
         <f aca="false">B77</f>
         <v>0.76</v>
       </c>
@@ -1981,12 +2672,16 @@
         <v>0.86</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>167</v>
+      </c>
+      <c r="G78" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B78)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="B79" s="0" t="n">
         <f aca="false">0.98*B76</f>
@@ -1998,12 +2693,16 @@
       <c r="D79" s="0" t="n">
         <v>-1</v>
       </c>
+      <c r="G79" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B79)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B80" s="7" t="n">
+      <c r="A80" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B80" s="9" t="n">
         <v>0.6</v>
       </c>
       <c r="C80" s="0" t="n">
@@ -2013,14 +2712,21 @@
         <v>-1</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>165</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="G80" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B80)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B81" s="8" t="n">
+        <v>171</v>
+      </c>
+      <c r="B81" s="10" t="n">
         <f aca="false">0.98*B78</f>
         <v>0.7448</v>
       </c>
@@ -2031,12 +2737,16 @@
         <v>-1</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>119</v>
+        <v>167</v>
+      </c>
+      <c r="G81" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B81)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>0.58</v>
@@ -2048,12 +2758,19 @@
         <v>0.7</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>162</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="G82" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B82)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="B83" s="0" t="n">
         <f aca="false">B79</f>
@@ -2066,12 +2783,16 @@
         <v>-1</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+      <c r="G83" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B83)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>126</v>
+        <v>176</v>
       </c>
       <c r="B84" s="0" t="n">
         <f aca="false">B79</f>
@@ -2084,14 +2805,18 @@
         <v>-1</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>125</v>
+        <v>175</v>
+      </c>
+      <c r="G84" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B84)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B85" s="4" t="n">
+        <v>177</v>
+      </c>
+      <c r="B85" s="7" t="n">
         <v>0.7</v>
       </c>
       <c r="C85" s="0" t="n">
@@ -2099,13 +2824,20 @@
       </c>
       <c r="D85" s="0" t="n">
         <v>-1</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="G85" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B85)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B86" s="3" t="n">
+        <v>179</v>
+      </c>
+      <c r="B86" s="6" t="n">
         <v>0.84</v>
       </c>
       <c r="C86" s="0" t="n">
@@ -2115,12 +2847,19 @@
         <v>-1</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="9" t="s">
-        <v>130</v>
+        <v>180</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="G86" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B86)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="11" t="s">
+        <v>182</v>
       </c>
       <c r="B87" s="0" t="n">
         <f aca="false">12/$B88</f>
@@ -2133,12 +2872,16 @@
         <v>-1</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>131</v>
+        <v>183</v>
+      </c>
+      <c r="G87" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B87)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="9" t="s">
-        <v>132</v>
+      <c r="A88" s="11" t="s">
+        <v>184</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>6</v>
@@ -2150,10 +2893,24 @@
         <v>-1</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>133</v>
+        <v>185</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="G88" s="4" t="n">
+        <f aca="false">_xlfn.ISFORMULA(B88)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G88">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2161,6 +2918,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2175,7 +2933,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2201,7 +2959,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.00049</v>
@@ -2213,12 +2971,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.612</v>
@@ -2230,14 +2988,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -2247,12 +3005,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.048</v>
@@ -2264,7 +3022,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2289,7 +3047,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2315,7 +3073,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.00049</v>
@@ -2327,12 +3085,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.597</v>
@@ -2344,14 +3102,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -2361,12 +3119,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.048</v>
@@ -2378,7 +3136,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2403,7 +3161,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2429,7 +3187,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.00049</v>
@@ -2441,12 +3199,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.581</v>
@@ -2458,14 +3216,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -2475,12 +3233,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.048</v>
@@ -2492,7 +3250,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2517,7 +3275,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2543,7 +3301,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.0071</v>
@@ -2555,12 +3313,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.735</v>
@@ -2572,14 +3330,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -2589,12 +3347,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.404</v>
@@ -2606,7 +3364,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2631,7 +3389,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2657,7 +3415,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.0071</v>
@@ -2669,12 +3427,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.72</v>
@@ -2686,14 +3444,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -2703,12 +3461,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.314</v>
@@ -2720,7 +3478,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2745,7 +3503,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2771,7 +3529,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.01058</v>
@@ -2783,12 +3541,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.704</v>
@@ -2800,14 +3558,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -2817,12 +3575,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.314</v>
@@ -2834,7 +3592,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2859,7 +3617,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2885,7 +3643,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.01058</v>
@@ -2897,12 +3655,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.689</v>
@@ -2914,14 +3672,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -2931,12 +3689,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.219</v>
@@ -2948,7 +3706,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2973,7 +3731,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -2999,7 +3757,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.00049</v>
@@ -3011,12 +3769,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.673</v>
@@ -3028,14 +3786,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -3045,12 +3803,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.219</v>
@@ -3062,7 +3820,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3087,7 +3845,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -3113,7 +3871,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.00049</v>
@@ -3125,12 +3883,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.658</v>
@@ -3142,14 +3900,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -3159,12 +3917,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.048</v>
@@ -3176,7 +3934,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3201,7 +3959,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -3227,7 +3985,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.00049</v>
@@ -3239,12 +3997,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.643</v>
@@ -3256,14 +4014,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -3273,12 +4031,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.048</v>
@@ -3290,7 +4048,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3315,7 +4073,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -3341,7 +4099,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.00049</v>
@@ -3353,12 +4111,12 @@
         <v>-1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.627</v>
@@ -3370,14 +4128,14 @@
         <v>-1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.001706</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -3387,12 +4145,12 @@
         <v>-1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.048</v>
@@ -3404,7 +4162,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add and fix issues for model review
</commit_message>
<xml_diff>
--- a/params/context.xlsx
+++ b/params/context.xlsx
@@ -22,7 +22,7 @@
     <sheet name="y80_84" sheetId="12" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">y25_29!$A$1:$F$92</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">y25_29!$A$1:$F$91</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="195">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -526,12 +526,6 @@
   </si>
   <si>
     <t xml:space="preserve">Probability of success in TCA for HSIL patients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hr_hsil_irc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assuming previous IRC does not prevent future HSILs</t>
   </si>
   <si>
     <t xml:space="preserve">u_hiv_p</t>
@@ -633,7 +627,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -672,7 +666,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -701,12 +695,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC55A11"/>
         <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -755,43 +743,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -804,7 +792,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -840,14 +828,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B0F0"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -895,7 +875,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00B0F0"/>
+      <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
@@ -1105,1692 +1085,1688 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="122.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="87.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="122.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="87.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>10.71</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">B6+0.67</f>
         <v>6.67</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <f aca="false">B6+0.67</f>
         <v>6.67</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <f aca="false">B6+0.67</f>
         <v>6.67</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="C6" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <f aca="false">B10</f>
         <v>71.25</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D7" s="0" t="n">
+      <c r="C7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <f aca="false">B10</f>
         <v>71.25</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D8" s="0" t="n">
+      <c r="C8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <f aca="false">B10</f>
         <v>71.25</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D9" s="0" t="n">
+      <c r="C9" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>71.25</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="C10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>20.02</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="C11" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="B12" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="C12" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <f aca="false">B12+B19</f>
         <v>31.6</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="C13" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <f aca="false">B12+B18</f>
         <v>103.70528</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="C14" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5" t="n">
+      <c r="B15" s="7" t="n">
         <v>82.05</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="C15" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="5" t="n">
+      <c r="B16" s="7" t="n">
         <v>30.56</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="C16" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="5" t="n">
+      <c r="B17" s="7" t="n">
         <v>75.04</v>
       </c>
-      <c r="C17" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="C17" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <f aca="false">B17*B22</f>
         <v>103.70528</v>
       </c>
-      <c r="C18" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D18" s="0" t="n">
+      <c r="C18" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>31.6</v>
       </c>
-      <c r="C19" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="C19" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>3189</v>
       </c>
-      <c r="C20" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="C20" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>3189</v>
       </c>
-      <c r="C21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="C21" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="5" t="n">
+      <c r="B22" s="7" t="n">
         <v>1.382</v>
       </c>
-      <c r="C22" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E22" s="4" t="s">
+      <c r="C22" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="3" t="n">
+      <c r="B23" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C23" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="C23" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="0" t="n">
-        <f aca="false">1-(1-B26)^(1/$B$91)</f>
+      <c r="B24" s="1" t="n">
+        <f aca="false">1-(1-B26)^(1/$B$90)</f>
         <v>0.000900641426546223</v>
       </c>
-      <c r="C24" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D24" s="0" t="n">
+      <c r="C24" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="6" t="n">
+      <c r="B25" s="8" t="n">
         <f aca="false">B24</f>
         <v>0.000900641426546223</v>
       </c>
-      <c r="C25" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E25" s="0" t="n">
+      <c r="C25" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E25" s="1" t="n">
         <v>0.001908</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <f aca="false">0.007634/4.24</f>
         <v>0.00180047169811321</v>
       </c>
-      <c r="C26" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="C26" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>0.4013</v>
       </c>
-      <c r="C27" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="C27" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>0.2792</v>
       </c>
-      <c r="C28" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="C28" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>0.2739</v>
       </c>
-      <c r="C29" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E29" s="0" t="s">
+      <c r="C29" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>0.6447</v>
       </c>
-      <c r="C30" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="C30" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>0.3057</v>
       </c>
-      <c r="C31" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D31" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="C31" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>0.0254</v>
       </c>
-      <c r="C32" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="C32" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <f aca="false">1-(1-EXP(-B73*5))^(1/$B$91)</f>
+      <c r="B33" s="1" t="n">
+        <f aca="false">1-(1-EXP(-B73*5))^(1/$B$90)</f>
         <v>0.0118288335799355</v>
       </c>
-      <c r="C33" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D33" s="0" t="n">
+      <c r="C33" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D33" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="6" t="n">
+      <c r="B34" s="8" t="n">
         <f aca="false">B33</f>
         <v>0.0118288335799355</v>
       </c>
-      <c r="C34" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D34" s="0" t="n">
+      <c r="C34" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D34" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="0" t="n">
-        <f aca="false">1-(1-B36)^(1/$B$91)</f>
+      <c r="B35" s="1" t="n">
+        <f aca="false">1-(1-B36)^(1/$B$90)</f>
         <v>0.000853364115156463</v>
       </c>
-      <c r="C35" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D35" s="0" t="n">
+      <c r="C35" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D35" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="6" t="n">
+      <c r="B36" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C36" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="C36" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>0.386</v>
       </c>
-      <c r="C37" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D37" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="C37" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F37" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <v>0.106</v>
       </c>
-      <c r="C38" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="C38" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <v>0.429</v>
       </c>
-      <c r="C39" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D39" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E39" s="0" t="s">
+      <c r="C39" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="1" t="n">
         <v>0.137</v>
       </c>
-      <c r="C40" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E40" s="0" t="s">
+      <c r="C40" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="1" t="n">
         <v>0.786</v>
       </c>
-      <c r="C41" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E41" s="0" t="s">
+      <c r="C41" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="F41" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <v>0.426</v>
       </c>
-      <c r="C42" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E42" s="0" t="s">
+      <c r="C42" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="F42" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <v>0.471</v>
       </c>
-      <c r="C43" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E43" s="0" t="s">
+      <c r="C43" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F43" s="0" t="s">
+      <c r="F43" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <v>0.173</v>
       </c>
-      <c r="C44" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E44" s="0" t="s">
+      <c r="C44" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="F44" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>0.549</v>
       </c>
-      <c r="C45" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D45" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E45" s="0" t="s">
+      <c r="C45" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="F45" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <v>0.294</v>
       </c>
-      <c r="C46" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D46" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E46" s="0" t="s">
+      <c r="C46" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="F46" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="1" t="n">
         <v>0.94</v>
       </c>
-      <c r="C47" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D47" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E47" s="0" t="s">
+      <c r="C47" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F47" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="1" t="n">
         <v>0.657</v>
       </c>
-      <c r="C48" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E48" s="0" t="s">
+      <c r="C48" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="F48" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B49" s="1" t="n">
         <v>0.757</v>
       </c>
-      <c r="C49" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E49" s="0" t="s">
+      <c r="C49" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="F49" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="1" t="n">
         <v>0.345</v>
       </c>
-      <c r="C50" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E50" s="0" t="s">
+      <c r="C50" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="F50" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="1" t="n">
         <v>0.8535</v>
       </c>
-      <c r="C51" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D51" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E51" s="0" t="s">
+      <c r="C51" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F51" s="0" t="s">
+      <c r="F51" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B52" s="3" t="n">
+      <c r="B52" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C52" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E52" s="4" t="s">
+      <c r="C52" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E52" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="6" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B53" s="0" t="n">
+      <c r="B53" s="1" t="n">
         <f aca="false">B51</f>
         <v>0.8535</v>
       </c>
-      <c r="C53" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E53" s="0" t="s">
+      <c r="C53" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="3" t="n">
+      <c r="B54" s="5" t="n">
         <f aca="false">B52</f>
         <v>0</v>
       </c>
-      <c r="C54" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D54" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E54" s="4" t="s">
+      <c r="C54" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B55" s="6" t="n">
+      <c r="B55" s="8" t="n">
         <f aca="false">B25</f>
         <v>0.000900641426546223</v>
       </c>
-      <c r="C55" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D55" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E55" s="4" t="s">
+      <c r="C55" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="6" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B56" s="3" t="n">
+      <c r="B56" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C56" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E56" s="4" t="s">
+      <c r="C56" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B57" s="6" t="n">
+      <c r="B57" s="8" t="n">
         <f aca="false">B55</f>
         <v>0.000900641426546223</v>
       </c>
-      <c r="C57" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D57" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E57" s="4" t="s">
+      <c r="C57" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B58" s="3" t="n">
+      <c r="B58" s="5" t="n">
         <f aca="false">B56</f>
         <v>0</v>
       </c>
-      <c r="C58" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D58" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E58" s="4" t="s">
+      <c r="C58" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D58" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B59" s="0" t="n">
-        <f aca="false">1-(1-B63)^(1/$B$91)</f>
+      <c r="B59" s="1" t="n">
+        <f aca="false">1-(1-B63)^(1/$B$90)</f>
         <v>0.227989637375249</v>
       </c>
-      <c r="C59" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D59" s="0" t="n">
+      <c r="C59" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D59" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="1" t="n">
         <f aca="false">B59</f>
         <v>0.227989637375249</v>
       </c>
-      <c r="C60" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D60" s="0" t="n">
+      <c r="C60" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D60" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B61" s="0" t="n">
+      <c r="B61" s="1" t="n">
         <f aca="false">B76*(1-B35)</f>
         <v>0.619470914248603</v>
       </c>
-      <c r="C61" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D61" s="0" t="n">
+      <c r="C61" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D61" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="0" t="n">
+      <c r="B62" s="1" t="n">
         <f aca="false">B77*(1-B35)</f>
         <v>0.617472620976833</v>
       </c>
-      <c r="C62" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D62" s="0" t="n">
+      <c r="C62" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D62" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="1" t="n">
         <v>0.404</v>
       </c>
-      <c r="C63" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D63" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E63" s="0" t="s">
+      <c r="C63" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F63" s="0" t="s">
+      <c r="F63" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="0" t="n">
-        <f aca="false">1-(1-B67)^(1/$B$91)</f>
+      <c r="B64" s="1" t="n">
+        <f aca="false">1-(1-B67)^(1/$B$90)</f>
         <v>0.0527935811028306</v>
       </c>
-      <c r="C64" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D64" s="0" t="n">
+      <c r="C64" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D64" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B65" s="0" t="n">
-        <f aca="false">1-EXP(-(-LOG(B69,EXP(1))/17.5)*1/$B$91)</f>
+      <c r="B65" s="1" t="n">
+        <f aca="false">1-EXP(-(-LOG(B69,EXP(1))/17.5)*1/$B$90)</f>
         <v>0.0295495344822225</v>
       </c>
-      <c r="C65" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D65" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E65" s="0" t="s">
+      <c r="C65" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B66" s="0" t="n">
+      <c r="B66" s="1" t="n">
         <f aca="false">B64</f>
         <v>0.0527935811028306</v>
       </c>
-      <c r="C66" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D66" s="0" t="n">
+      <c r="C66" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D66" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="1" t="n">
         <v>0.1028</v>
       </c>
-      <c r="C67" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D67" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E67" s="0" t="s">
+      <c r="C67" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D67" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F67" s="0" t="s">
+      <c r="F67" s="1" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B68" s="0" t="n">
+      <c r="B68" s="1" t="n">
         <f aca="false">B65</f>
         <v>0.0295495344822225</v>
       </c>
-      <c r="C68" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D68" s="0" t="n">
+      <c r="C68" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D68" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B69" s="0" t="n">
+      <c r="B69" s="1" t="n">
         <v>0.35</v>
       </c>
-      <c r="C69" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D69" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E69" s="0" t="s">
+      <c r="C69" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D69" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F69" s="0" t="s">
+      <c r="F69" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B70" s="3" t="n">
-        <f aca="false">1-(1-B71)^(1/$B$91)</f>
+      <c r="B70" s="5" t="n">
+        <f aca="false">1-(1-B71)^(1/$B$90)</f>
         <v>0</v>
       </c>
-      <c r="C70" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D70" s="0" t="n">
+      <c r="C70" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D70" s="1" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B71" s="3" t="n">
+      <c r="B71" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C71" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D71" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E71" s="4" t="s">
+      <c r="C71" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D71" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F71" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B72" s="3" t="n">
+      <c r="B72" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="C72" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D72" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E72" s="4" t="s">
+      <c r="C72" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D72" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F72" s="6" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B73" s="0" t="n">
+      <c r="B73" s="1" t="n">
         <v>0.75</v>
       </c>
-      <c r="C73" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D73" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E73" s="0" t="s">
+      <c r="C73" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D73" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F73" s="0" t="s">
+      <c r="F73" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B74" s="3" t="n">
+      <c r="B74" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C74" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D74" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E74" s="4" t="s">
+      <c r="C74" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D74" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="F74" s="6" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B75" s="3" t="n">
+      <c r="B75" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C75" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D75" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E75" s="4" t="s">
+      <c r="C75" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D75" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="F75" s="6" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B76" s="5" t="n">
+      <c r="B76" s="7" t="n">
         <v>0.62</v>
       </c>
-      <c r="C76" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D76" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E76" s="4" t="s">
+      <c r="C76" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D76" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F76" s="4" t="s">
+      <c r="F76" s="6" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B77" s="5" t="n">
+      <c r="B77" s="7" t="n">
         <v>0.618</v>
       </c>
-      <c r="C77" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D77" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E77" s="4" t="s">
+      <c r="C77" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D77" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F77" s="4" t="s">
+      <c r="F77" s="6" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B78" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C78" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D78" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E78" s="4" t="s">
+      <c r="B78" s="6" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F78" s="4" t="s">
-        <v>150</v>
+      <c r="F78" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B79" s="7" t="n">
+      <c r="A79" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B79" s="6" t="n">
+        <f aca="false">B78</f>
         <v>0.84</v>
       </c>
-      <c r="C79" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D79" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="F79" s="4" t="s">
+      <c r="C79" s="1" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B80" s="6" t="n">
         <f aca="false">B79</f>
         <v>0.84</v>
       </c>
-      <c r="C80" s="0" t="n">
+      <c r="C80" s="1" t="n">
         <v>0.66</v>
       </c>
-      <c r="D80" s="0" t="n">
+      <c r="D80" s="1" t="n">
         <v>0.86</v>
       </c>
-      <c r="E80" s="4" t="s">
+      <c r="E80" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B81" s="6" t="n">
-        <f aca="false">B80</f>
+      <c r="B81" s="1" t="n">
+        <f aca="false">0.98*B78</f>
+        <v>0.8232</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B82" s="6" t="n">
+        <v>0.835</v>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D82" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" s="1" t="n">
+        <v>0.836</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D83" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B84" s="1" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D84" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B85" s="1" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D85" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B86" s="1" t="n">
+        <f aca="false">B81</f>
+        <v>0.8232</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D86" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B87" s="1" t="n">
+        <f aca="false">B81</f>
+        <v>0.8232</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D87" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B88" s="1" t="n">
         <v>0.84</v>
       </c>
-      <c r="C81" s="0" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="D81" s="0" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B82" s="0" t="n">
-        <f aca="false">0.98*B79</f>
-        <v>0.8232</v>
-      </c>
-      <c r="C82" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D82" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B83" s="8" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C83" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D83" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="B84" s="9" t="n">
-        <f aca="false">0.98*B81</f>
-        <v>0.8232</v>
-      </c>
-      <c r="C84" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D84" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B85" s="0" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="C85" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D85" s="0" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="E85" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="F85" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B86" s="0" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="C86" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D86" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E86" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="F86" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B87" s="0" t="n">
-        <f aca="false">B82</f>
-        <v>0.8232</v>
-      </c>
-      <c r="C87" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D87" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E87" s="0" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="C88" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D88" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B88" s="0" t="n">
-        <f aca="false">B82</f>
-        <v>0.8232</v>
-      </c>
-      <c r="C88" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D88" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E88" s="0" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="89" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B89" s="5" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="C89" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D89" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F89" s="4" t="s">
+      <c r="B89" s="6" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D89" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="F89" s="1" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B90" s="6" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="C90" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D90" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E90" s="4" t="s">
+      <c r="A90" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="F90" s="4" t="s">
+      <c r="B90" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D90" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2798,42 +2774,26 @@
       <c r="A91" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="B91" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C91" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D91" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E91" s="4" t="s">
+      <c r="B91" s="6" t="n">
+        <f aca="false">12/B90</f>
+        <v>6</v>
+      </c>
+      <c r="C91" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D91" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="10" t="s">
+      <c r="F91" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B92" s="4" t="n">
-        <f aca="false">12/B91</f>
-        <v>6</v>
-      </c>
-      <c r="C92" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D92" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F92"/>
+  <autoFilter ref="A1:F91"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2858,93 +2818,93 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.00184691109687812</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.612</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.048</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2972,93 +2932,93 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.0018916537948187</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.597</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.048</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3086,94 +3046,94 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <f aca="false">0.007634/4.24</f>
         <v>0.00180047169811321</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.581</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.048</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3201,94 +3161,94 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <f aca="false">0.007634/4.24</f>
         <v>0.00180047169811321</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.735</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.404</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3310,100 +3270,100 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <f aca="false">0.007634/4.24</f>
         <v>0.00180047169811321</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.72</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.314</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3426,98 +3386,98 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.0058691355195081</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>196</v>
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.704</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.314</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3540,98 +3500,98 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.00344980252811424</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.689</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.219</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3659,93 +3619,93 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.00324775583133558</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.673</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.219</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3768,98 +3728,98 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="E74" activeCellId="0" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.00258766335262408</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.658</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.048</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3887,93 +3847,93 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.00193687668776452</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.643</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.048</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4001,93 +3961,93 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>0.0018456703895995</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>0.627</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="8" t="n">
         <v>0.001706</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.048</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>